<commit_message>
Naive Bayes Testing implemented
</commit_message>
<xml_diff>
--- a/Configurations/TestResults.xlsx
+++ b/Configurations/TestResults.xlsx
@@ -12,6 +12,7 @@
     <sheet name="CompleteSVM2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="CompleteSVM3" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CompleteSVM4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CompleteNB" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -679,4 +680,46 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f1_score</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>